<commit_message>
Refine functionality + tests for 100% coverage.
Signed-off-by: degenaro <lou.degenaro@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/data/tasks/cis-xlsx-to-oscal-catalog/CIS_RedHat_OpenShift_Container_Platform_Benchmark_v1.2.0-2.snippet.xlsx
+++ b/tests/data/tasks/cis-xlsx-to-oscal-catalog/CIS_RedHat_OpenShift_Container_Platform_Benchmark_v1.2.0-2.snippet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="102">
   <si>
     <t xml:space="preserve">section #</t>
   </si>
@@ -353,6 +353,110 @@
   </si>
   <si>
     <t xml:space="preserve">https://docs.openshift.com/container-platform/4.3/architecture/control-plane.html#defining-masters_control-plane:https://github.com/openshift/cluster-etcd-operator/blob/master/bindata/etcd/pod.yaml:https://etcd.io/:https://kubernetes.io/docs/tasks/administer-cluster/configure-upgrade-etcd/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section contains recommendations relating to API server configuration flags. 
+OpenShift includes two API servers, the OpenShift API server and the Kubernetes API server. All API calls are directed to the Open Shift API server and then Kubernetes objects are delegated to `kube-apiserver`.
+The cluster configuration resource (CR) APIServer holds configuration settings (like serving certificates, client CA and CORS domains) shared by all API servers in the system, among them especially `kube-apiserver` and `openshift-apiserver`. The canonical name of an instance is 'cluster'. Changes to the API server configurations should be done in the APIServer custom resource definition (CRD): apiservers.config.openshift.io
+The OpenShift API Server is managed by the `openshift-apiserver-operator`
+The Kubernetes API Server is managed by the `openshift-kube-apiserver-operator`
+Both are managed by the Cluster Version Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure that anonymous requests are authorized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When anonymous requests to the API server are allowed, they must be authorized.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When enabled, requests that are not rejected by other configured authentication methods are treated as anonymous requests. These requests are then served by the API server. You should rely on authentication to authorize anonymous requests.
+If you are using RBAC authorization, it is generally considered reasonable to allow anonymous access to the API Server for health checks and discovery purposes, and hence this recommendation is not scored. However, you should consider whether anonymous discovery is an acceptable risk for your purposes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anonymous requests are assigned to the `system:unauthenticated` group which allows the system to determine which actions are allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None required. The default configuration should not be modified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenShift allows anonymous requests (then authorizes them). OpenShift allows anonymous requests to the API server to support information discovery and `webhook` integrations. OpenShift provides it's own fully integrated authentication and authorization mechanism. If no access token or certificate is presented, the authentication layer assigns the `system:anonymous` virtual user and the `system:unauthenticated` virtual group to the request. This allows the authorization layer to determine which requests, if any, an anonymous user is allowed to make.
+```
+# To verify that userGroups include system:unauthenticated
+oc get configmap config -n openshift-kube-apiserver -ojson | \
+ jq -r '.data["config.yaml"]' | \
+ jq '.auditConfig.policyConfiguration.rules[]'
+# To verify that userGroups include system:unauthenticated
+oc get configmap config -n openshift-apiserver -ojson | \
+ jq -r '.data["config.yaml"]' | \
+ jq '.auditConfig.policyConfiguration.rules[]'
+# To verify RBAC is enabled
+oc get clusterrolebinding
+oc get clusterrole
+oc get rolebinding
+oc get role
+```
+Verify that the userGroups include `system:unauthenticated`.
+Verify that role bindings and roles are returned.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA0001, TA0008, T1190, T1210, M1025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.openshift.com/container-platform/4.5/authentication/understanding-authentication.html:https://docs.openshift.com/container-platform/4.5/authentication/using-rbac.html:https://docs.openshift.com/container-platform/4.5/operators/operator-reference.html#cluster-authentication-operator_red-hat-operators:https://docs.openshift.com/container-platform/4.5/operators/operator-reference.html#kube-apiserver-operator_red-hat-operators:https://docs.openshift.com/container-platform/4.5/operators/operator-reference.html#openshift-apiserver-operator_red-hat-operators:https://kubernetes.io/docs/reference/command-line-tools-reference/kube-apiserver/:https://kubernetes.io/docs/reference/access-authn-authz/authentication/#anonymous-requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use https for kubelet connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use https for kubelet connections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connections from `apiserver` to `kubelets` could potentially carry sensitive data such as secrets and keys. It is thus important to use in-transit encryption for any communication between the `apiserver` and `kubelets`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You require TLS to be configured on `apiserver` as well as `kubelets`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No remediation is required. OpenShift platform components use X.509 certificates for authentication. OpenShift manages the CAs and certificates for platform components. This is not configurable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenShift does not use the `--kubelet-https` argument. OpenShift utilizes X.509 certificates for authentication of the control-plane components. OpenShift configures the API server to use an internal certificate authority (CA) to validate the user certificate sent during TLS negotiation. If the validation of the certificate is successful, the request is authenticated and user information is derived from the certificate subject fields.
+To verify the kubelet client certificates are present, run the following command:
+```
+#for 4.5
+oc get configmap config -n openshift-kube-apiserver -ojson | jq -r '.data["config.yaml"]' | jq '.kubeletClientInfo' 
+#for 4.6
+oc get configmap config -n openshift-kube-apiserver -ojson | jq -r '.data["config.yaml"]' | jq '.apiServerArguments'
+#for both 4.5 and 4.6
+oc -n openshift-apiserver describe secret serving-cert
+```
+Verify that the kubelet client-certificate and kubelet client-key files are present.
+client-certificate: 
+`/etc/kubernetes/static-pod-resources/secrets/kubelet-client/tls.crt`
+client-key: 
+`/etc/kubernetes/static-pod-resources/secrets/kubelet-client/tls.key`
+Verify that the serving-cert for the `openshift-apiserver` is type kubernetes.io/tls and that returned Data includes `tls.crt` and `tls.key`.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TITLE:Encrypt Sensitive Data in Transit CONTROL:v8 3.10 DESCRIPTION:Encrypt sensitive data in transit. Example implementations can include: Transport Layer Security (TLS) and Open Secure Shell (OpenSSH).;TITLE:Encrypt All Sensitive Information in Transit CONTROL:v7 14.4 DESCRIPTION:Encrypt all sensitive information in transit.;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA0001, TA0010, T1048, T1189, M1041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.openshift.com/container-platform/4.5/operators/operator-reference.html#kube-apiserver-operator_red-hat-operators:https://docs.openshift.com/container-platform/4.5/operators/operator-reference.html#openshift-apiserver-operator_red-hat-operators:https://github.com/openshift/cluster-kube-apiserver-operator/blob/release-4.5/bindata/v4.1.0/config/defaultconfig.yaml#L12-L13:https://github.com/openshift/cluster-kube-apiserver-operator/blob/release-4.5/bindata/v4.1.0/config/defaultconfig.yaml#L94-L98:https://kubernetes.io/docs/reference/command-line-tools-reference/kube-apiserver/:https://kubernetes.io/docs/reference/command-line-tools-reference/kubelet-authentication-authorization/</t>
   </si>
 </sst>
 </file>
@@ -608,17 +712,17 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="13:13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="6" style="0" width="15"/>
   </cols>
@@ -1200,6 +1304,162 @@
       <c r="U10" s="3"/>
       <c r="V10" s="3" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>